<commit_message>
update battle service, add trading service
</commit_message>
<xml_diff>
--- a/documentation/specification/Checklist.xlsx
+++ b/documentation/specification/Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fhtw-my.sharepoint.com/personal/if21b054_technikum-wien_at/Documents/BIF/3_Semester/SWEN1/Projekte/MonsterTradingCardGame/documentation/specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{6654F465-E96B-4F58-9905-119C7AA41DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39C59A80-57C8-485D-BB2D-C0DC235F0140}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="13_ncr:1_{6654F465-E96B-4F58-9905-119C7AA41DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D37321E-22F4-46F2-8696-B5AAC7E134A9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{88369686-F968-45CB-887F-E38F2E727DD7}"/>
   </bookViews>
@@ -611,7 +611,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D58600B0-3567-4A3D-A785-925E0537D06D}">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -844,6 +846,9 @@
       <c r="A32" s="6" t="s">
         <v>27</v>
       </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
       <c r="C32" s="6">
         <v>2</v>
       </c>
@@ -862,6 +867,9 @@
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>29</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
       </c>
       <c r="C34" s="6">
         <v>2</v>
@@ -1013,21 +1021,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100495F7CC252815B47896F98900E10984C" ma:contentTypeVersion="2" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="afe1b3b164495dc81fdbcdcad6ec8b68">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="207955a2-a3fc-4582-b2ea-e4c7d1fb6048" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b6a42bf87c3f8727d31c248fc1697f6" ns2:_="">
     <xsd:import namespace="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
@@ -1159,31 +1152,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FFD0135-03B1-4A6A-9DC8-B4D791C0671E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B871BF9-5772-4B74-B6DF-7878EF29873D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0824ED0-660A-437B-A039-7835C5DD208D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1199,4 +1183,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B871BF9-5772-4B74-B6DF-7878EF29873D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FFD0135-03B1-4A6A-9DC8-B4D791C0671E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add unique logout feature
</commit_message>
<xml_diff>
--- a/documentation/specification/Checklist.xlsx
+++ b/documentation/specification/Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fhtw-my.sharepoint.com/personal/if21b054_technikum-wien_at/Documents/BIF/3_Semester/SWEN1/Projekte/MonsterTradingCardGame/documentation/specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="13_ncr:1_{6654F465-E96B-4F58-9905-119C7AA41DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5823816-990B-424D-9B14-A268E13E69D2}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="13_ncr:1_{6654F465-E96B-4F58-9905-119C7AA41DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A6129848-91A2-4B96-8D4C-E556086CDEDD}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{88369686-F968-45CB-887F-E38F2E727DD7}"/>
   </bookViews>
@@ -714,7 +714,7 @@
         <v>12</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.4">
@@ -880,6 +880,9 @@
       <c r="A36" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="B36" s="1">
+        <v>3</v>
+      </c>
       <c r="C36" s="6">
         <v>3</v>
       </c>
@@ -916,6 +919,9 @@
       <c r="A41" s="6" t="s">
         <v>34</v>
       </c>
+      <c r="B41">
+        <v>5</v>
+      </c>
       <c r="C41" s="6">
         <v>5</v>
       </c>
@@ -1003,7 +1009,7 @@
       </c>
       <c r="B54" s="2">
         <f>IF(MIN(B9:B16)=1,SUM(B21:B52),0)</f>
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="C54" s="2">
         <f>SUM(C21:C52)</f>

</xml_diff>